<commit_message>
add easyloggin++; add award/drop pack module; add log configure file for win & linux; add some config in npc & item;
Former-commit-id: dcbf023e3d84790a4e2d78cecc35258ccda6d00f [formerly 70cf388193254a4aaf86e6c8f793d3b609334406]
Former-commit-id: 1ade227796daba80cbda66d86020e9214c765009
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>QDJL-JB</t>
+  </si>
+  <si>
+    <t>Equip_Weapon_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开山斧</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开山斧武器</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50004</t>
   </si>
 </sst>
 </file>
@@ -231,8 +246,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K8" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:K8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:K9" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:K9"/>
   <tableColumns count="11">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
@@ -535,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -835,6 +850,41 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>10000</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix Item Id -> ID
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
@@ -76,9 +76,6 @@
     <t>50004</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t>ItemType</t>
   </si>
   <si>
@@ -224,6 +221,10 @@
   </si>
   <si>
     <t>Prefabs/Item/Equip_Weapon_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -338,7 +339,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:AC9" tableType="xml" totalsRowShown="0" connectionId="1">
   <autoFilter ref="A1:AC9"/>
   <tableColumns count="29">
-    <tableColumn id="1" uniqueName="ID" name="Id">
+    <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="ItemType" name="ItemType">
@@ -659,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -695,96 +696,96 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>26</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>28</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>31</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>40</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>41</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>42</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -817,12 +818,12 @@
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -855,12 +856,12 @@
         <v>0</v>
       </c>
       <c r="V3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -893,12 +894,12 @@
         <v>0</v>
       </c>
       <c r="V4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -931,12 +932,12 @@
         <v>0</v>
       </c>
       <c r="V5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -969,12 +970,12 @@
         <v>0</v>
       </c>
       <c r="V6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1007,12 +1008,12 @@
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1045,12 +1046,12 @@
         <v>0</v>
       </c>
       <c r="V8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1083,7 +1084,7 @@
         <v>100</v>
       </c>
       <c r="V9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redesign the item system
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Item.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\NoahGameFrame\_Out\Server\NFDataCfg\Excel_Ini\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>钱盒子</t>
   </si>
@@ -50,32 +50,10 @@
     <t>活动令牌</t>
   </si>
   <si>
-    <t>装了好多钱</t>
-  </si>
-  <si>
-    <t>1017</t>
-  </si>
-  <si>
-    <t>1018</t>
-  </si>
-  <si>
-    <t>1019</t>
-  </si>
-  <si>
-    <t>QDJL-JB</t>
-  </si>
-  <si>
     <t>开山斧</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>开山斧武器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50004</t>
-  </si>
-  <si>
     <t>ItemType</t>
   </si>
   <si>
@@ -91,60 +69,15 @@
     <t>Quality</t>
   </si>
   <si>
-    <t>Bound</t>
-  </si>
-  <si>
-    <t>ShowName</t>
-  </si>
-  <si>
-    <t>Desc</t>
-  </si>
-  <si>
-    <t>EffectProperty</t>
-  </si>
-  <si>
-    <t>EffectValue</t>
-  </si>
-  <si>
     <t>EffectData</t>
   </si>
   <si>
-    <t>ActiveEffectData</t>
-  </si>
-  <si>
-    <t>ActiveEffectDataPercent</t>
-  </si>
-  <si>
-    <t>Icon</t>
-  </si>
-  <si>
-    <t>Atlas</t>
-  </si>
-  <si>
-    <t>GetItemList</t>
-  </si>
-  <si>
-    <t>GetBuffList</t>
-  </si>
-  <si>
-    <t>GetSkill</t>
-  </si>
-  <si>
     <t>CoolDownTime</t>
   </si>
   <si>
     <t>OverlayCount</t>
   </si>
   <si>
-    <t>PrefabPath</t>
-  </si>
-  <si>
-    <t>PerformanceEffect</t>
-  </si>
-  <si>
-    <t>PerformanceSound</t>
-  </si>
-  <si>
     <t>ExpiredType</t>
   </si>
   <si>
@@ -157,74 +90,59 @@
     <t>Script</t>
   </si>
   <si>
-    <t>Duration</t>
-  </si>
-  <si>
     <t>Item_Cash_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Item_Cash_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Item_HP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Item_HP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Item_MP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Item_MP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Item_EXP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Item_EXP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Item_New_Award</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Item_New_Award</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Gold_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Gold_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Active_Token</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Active_Token</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Equip_Weapon_1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Prefabs/Item/Equip_Weapon_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DescID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConsumeData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AwardData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DesignDesc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -336,9 +254,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:AC9" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:AC9"/>
-  <tableColumns count="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:R9" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:R9"/>
+  <tableColumns count="18">
     <tableColumn id="1" uniqueName="ID" name="ID">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
     </tableColumn>
@@ -357,39 +275,22 @@
     <tableColumn id="6" uniqueName="Desc" name="Quality">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@Desc" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="Icon" name="Bound">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@Icon" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="8" uniqueName="CoolDownTime" name="ShowName" dataDxfId="1">
+    <tableColumn id="8" uniqueName="CoolDownTime" name="DesignDesc" dataDxfId="1">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@CoolDownTime" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="OverlayCount" name="Desc" dataDxfId="0">
+    <tableColumn id="9" uniqueName="OverlayCount" name="DescID" dataDxfId="0">
       <xmlColumnPr mapId="1" xpath="/XML/Object/@OverlayCount" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="BuyPrice" name="EffectProperty">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@BuyPrice" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="11" uniqueName="SalePrice" name="EffectValue">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@SalePrice" xmlDataType="integer"/>
-    </tableColumn>
     <tableColumn id="12" uniqueName="12" name="EffectData"/>
-    <tableColumn id="13" uniqueName="13" name="ActiveEffectData"/>
-    <tableColumn id="14" uniqueName="14" name="ActiveEffectDataPercent"/>
-    <tableColumn id="15" uniqueName="15" name="Icon"/>
-    <tableColumn id="16" uniqueName="16" name="Atlas"/>
-    <tableColumn id="17" uniqueName="17" name="GetItemList"/>
-    <tableColumn id="18" uniqueName="18" name="GetBuffList"/>
-    <tableColumn id="19" uniqueName="19" name="GetSkill"/>
+    <tableColumn id="13" uniqueName="13" name="ConsumeData"/>
+    <tableColumn id="14" uniqueName="14" name="AwardData"/>
     <tableColumn id="20" uniqueName="20" name="CoolDownTime"/>
     <tableColumn id="21" uniqueName="21" name="OverlayCount"/>
-    <tableColumn id="22" uniqueName="22" name="PrefabPath"/>
-    <tableColumn id="23" uniqueName="23" name="PerformanceEffect"/>
-    <tableColumn id="24" uniqueName="24" name="PerformanceSound"/>
     <tableColumn id="25" uniqueName="25" name="ExpiredType"/>
     <tableColumn id="26" uniqueName="26" name="BuyPrice"/>
     <tableColumn id="27" uniqueName="27" name="SalePrice"/>
     <tableColumn id="28" uniqueName="28" name="Script"/>
-    <tableColumn id="29" uniqueName="29" name="Duration"/>
+    <tableColumn id="29" uniqueName="29" name="Extend"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AC14" sqref="AC14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -672,120 +573,78 @@
     <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="R1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" t="s">
-        <v>32</v>
-      </c>
-      <c r="T1" t="s">
-        <v>33</v>
-      </c>
-      <c r="U1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -803,45 +662,31 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>999</v>
       </c>
-      <c r="V2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>100</v>
-      </c>
-      <c r="AA2">
-        <v>100</v>
-      </c>
-      <c r="AC2">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>100</v>
+      </c>
+      <c r="P2">
+        <v>100</v>
+      </c>
+      <c r="R2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -859,45 +704,31 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>999</v>
       </c>
-      <c r="V3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3">
-        <v>0</v>
-      </c>
-      <c r="Z3">
-        <v>100</v>
-      </c>
-      <c r="AA3">
-        <v>100</v>
-      </c>
-      <c r="AC3">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="R3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -915,45 +746,31 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
+      <c r="H4" s="1"/>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>999</v>
       </c>
-      <c r="V4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4">
-        <v>100</v>
-      </c>
-      <c r="AA4">
-        <v>100</v>
-      </c>
-      <c r="AC4">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="R4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -971,45 +788,31 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
+      <c r="H5" s="1"/>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>999</v>
       </c>
-      <c r="V5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5">
-        <v>100</v>
-      </c>
-      <c r="AA5">
-        <v>100</v>
-      </c>
-      <c r="AC5">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="R5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1027,45 +830,31 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
+      <c r="H6" s="1"/>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>999</v>
       </c>
-      <c r="V6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>100</v>
-      </c>
-      <c r="AA6">
-        <v>100</v>
-      </c>
-      <c r="AC6">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>100</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="R6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1083,45 +872,31 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7">
+      <c r="H7" s="1"/>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
         <v>999</v>
       </c>
-      <c r="V7" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7">
-        <v>100</v>
-      </c>
-      <c r="AA7">
-        <v>100</v>
-      </c>
-      <c r="AC7">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>100</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="R7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1139,45 +914,31 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
+      <c r="H8" s="1"/>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>999</v>
       </c>
-      <c r="V8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8">
-        <v>100</v>
-      </c>
-      <c r="AA8">
-        <v>100</v>
-      </c>
-      <c r="AC8">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>100</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="R8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1194,40 +955,25 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9">
-        <v>100</v>
-      </c>
-      <c r="T9">
-        <v>1</v>
-      </c>
-      <c r="U9">
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
         <v>999</v>
       </c>
-      <c r="V9" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9">
-        <v>100</v>
-      </c>
-      <c r="AA9">
-        <v>100</v>
-      </c>
-      <c r="AC9">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="R9">
         <v>0</v>
       </c>
     </row>

</xml_diff>